<commit_message>
aggiunta mappatura intensità, da decidere come considerare l'itnensità della mappatura
</commit_message>
<xml_diff>
--- a/Docum/formule intensità.xlsx
+++ b/Docum/formule intensità.xlsx
@@ -16,17 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -47,12 +37,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -67,9 +63,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -371,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,7 +381,7 @@
     <col min="9" max="9" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -392,8 +389,8 @@
         <v>7</v>
       </c>
       <c r="C1" s="1">
-        <f>100-$D$11*A1</f>
-        <v>86</v>
+        <f>100-$D$11*A1+$D$11</f>
+        <v>100</v>
       </c>
       <c r="D1">
         <v>1</v>
@@ -402,7 +399,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1">
-        <f>E1/D1</f>
+        <f t="shared" ref="F1:F7" si="0">E1/D1</f>
         <v>3</v>
       </c>
       <c r="G1">
@@ -412,18 +409,15 @@
         <v>4</v>
       </c>
       <c r="I1" s="1">
-        <f>H1/G1</f>
+        <f t="shared" ref="I1:I7" si="1">H1/G1</f>
         <v>4</v>
       </c>
       <c r="J1">
-        <f>C1+$D$11*E1/D1</f>
-        <v>128</v>
-      </c>
-      <c r="K1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <f>(C1*E1/D1)+(C1*H1/G1)</f>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -431,8 +425,8 @@
         <v>7</v>
       </c>
       <c r="C2" s="1">
-        <f>100-$D$11*A2</f>
-        <v>72</v>
+        <f>100-$D$11*A2+$D$11</f>
+        <v>86</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -441,7 +435,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="1">
-        <f>E2/D2</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G2">
@@ -451,27 +445,28 @@
         <v>4</v>
       </c>
       <c r="I2" s="1">
-        <f>H2/G2</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J2">
-        <f>C2+$D$11*E2/D2</f>
-        <v>114</v>
-      </c>
-      <c r="K2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <f>$J$1*C2/100</f>
+        <v>602</v>
+      </c>
+      <c r="K2">
+        <f>ROUND(J2*100/J1,0)</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
-        <f>100-$D$11*A3</f>
-        <v>58</v>
+      <c r="C3" s="2">
+        <f>100-$D$11*A3+$D$11</f>
+        <v>72</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -480,7 +475,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="1">
-        <f>E3/D3</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G3">
@@ -490,18 +485,19 @@
         <v>4</v>
       </c>
       <c r="I3" s="1">
-        <f>H3/G3</f>
+        <f t="shared" si="1"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="J3">
-        <f>C3+$D$11*E3/D3</f>
-        <v>100</v>
-      </c>
-      <c r="K3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <f>$J$1*C3/100</f>
+        <v>504</v>
+      </c>
+      <c r="K3">
+        <f>ROUND(J3*100/J2,0)</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -509,8 +505,8 @@
         <v>7</v>
       </c>
       <c r="C4" s="1">
-        <f>100-$D$11*A4</f>
-        <v>44</v>
+        <f>100-$D$11*A4+$D$11</f>
+        <v>58</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -519,7 +515,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="1">
-        <f>E4/D4</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G4">
@@ -529,27 +525,28 @@
         <v>4</v>
       </c>
       <c r="I4" s="1">
-        <f>H4/G4</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J4">
-        <f>C4+$D$11*E4/D4</f>
-        <v>86</v>
-      </c>
-      <c r="K4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <f>$J$1*C4/100</f>
+        <v>406</v>
+      </c>
+      <c r="K4">
+        <f>ROUND(J4*100/J3,0)</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5">
         <v>7</v>
       </c>
-      <c r="C5" s="1">
-        <f>100-$D$11*A5</f>
-        <v>30</v>
+      <c r="C5" s="2">
+        <f>100-$D$11*A5+$D$11</f>
+        <v>44</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -558,7 +555,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="1">
-        <f>E5/D5</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="G5">
@@ -568,18 +565,22 @@
         <v>2</v>
       </c>
       <c r="I5" s="1">
-        <f>H5/G5</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J5">
-        <f>C5+$D$11*E5/D5</f>
-        <v>51</v>
-      </c>
-      <c r="K5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <f>($J$1*C5/100)</f>
+        <v>308</v>
+      </c>
+      <c r="K5">
+        <f>ROUND(J5*100/J4,0)</f>
+        <v>76</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -587,48 +588,49 @@
         <v>7</v>
       </c>
       <c r="C6" s="1">
-        <f>100-$D$11*A6</f>
+        <f>100-$D$11*A6+$D$11</f>
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <f>$J$1*C6/100</f>
+        <v>210</v>
+      </c>
+      <c r="K6">
+        <f>ROUND(J6*100/J5,0)</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1">
+        <f>100-$D$11*A7+$D$11</f>
         <v>16</v>
       </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6" s="1">
-        <f>E6/D6</f>
-        <v>1.5</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6" s="1">
-        <f>H6/G6</f>
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <f>C6+$D$11*E6/D6</f>
-        <v>37</v>
-      </c>
-      <c r="K6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1">
-        <f>100-$D$11*A7</f>
-        <v>2</v>
-      </c>
       <c r="D7">
         <v>3</v>
       </c>
@@ -636,7 +638,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="1">
-        <f>E7/D7</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G7">
@@ -646,18 +648,24 @@
         <v>1</v>
       </c>
       <c r="I7" s="1">
-        <f>H7/G7</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J7">
-        <f>C7+$D$11*E7/D7</f>
-        <v>16</v>
-      </c>
-      <c r="K7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <f>(($J$1*C7/100)*H7)</f>
+        <v>112</v>
+      </c>
+      <c r="K7">
+        <f>ROUND(J7*100/J6,0)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>100</v>
       </c>
@@ -668,8 +676,15 @@
         <f>ROUND(B11/C11,0)</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>66</v>
+      </c>
+      <c r="M11">
+        <f>K11*100/K10</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
         <f>B11/C11</f>
         <v>14.285714285714286</v>

</xml_diff>